<commit_message>
updated Copy of Face recognition Dev Plan
</commit_message>
<xml_diff>
--- a/Copy of Face recognition Dev Plan_v1 (2).xlsx
+++ b/Copy of Face recognition Dev Plan_v1 (2).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
   <si>
     <t>Functionality</t>
   </si>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,7 +1537,9 @@
       <c r="I37" s="9">
         <v>42221</v>
       </c>
-      <c r="J37" s="3"/>
+      <c r="J37" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
@@ -1555,7 +1557,9 @@
       <c r="I38" s="9">
         <v>42223</v>
       </c>
-      <c r="J38" s="3"/>
+      <c r="J38" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
@@ -1892,6 +1896,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F29:F35"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C39:C52"/>
+    <mergeCell ref="D39:D52"/>
+    <mergeCell ref="E39:E52"/>
+    <mergeCell ref="C30:C35"/>
+    <mergeCell ref="D30:D35"/>
+    <mergeCell ref="E30:E35"/>
     <mergeCell ref="C18:C23"/>
     <mergeCell ref="D18:D23"/>
     <mergeCell ref="E18:E23"/>
@@ -1901,14 +1913,6 @@
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="E15:E17"/>
-    <mergeCell ref="F29:F35"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C39:C52"/>
-    <mergeCell ref="D39:D52"/>
-    <mergeCell ref="E39:E52"/>
-    <mergeCell ref="C30:C35"/>
-    <mergeCell ref="D30:D35"/>
-    <mergeCell ref="E30:E35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>